<commit_message>
backend: Excel import -> incorrect counting of updated users (non-changed users were counted as updated ones when importing)
</commit_message>
<xml_diff>
--- a/users_app/test_data/import_template_EXAMPLE.xlsx
+++ b/users_app/test_data/import_template_EXAMPLE.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="516">
   <si>
     <t xml:space="preserve">email</t>
   </si>
@@ -688,10 +688,13 @@
     <t xml:space="preserve">Alice	Smith</t>
   </si>
   <si>
-    <t xml:space="preserve">alice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alice	Smith</t>
+    <t xml:space="preserve">alice.smith1@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alice.smith1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alice Smith</t>
   </si>
   <si>
     <t xml:space="preserve">bob.smith@example.com</t>
@@ -703,7 +706,7 @@
     <t xml:space="preserve">Bob</t>
   </si>
   <si>
-    <t xml:space="preserve">Bob	Smith</t>
+    <t xml:space="preserve">Bob Smith</t>
   </si>
   <si>
     <t xml:space="preserve">charlie.smith@example.com</t>
@@ -715,7 +718,7 @@
     <t xml:space="preserve">Charlie</t>
   </si>
   <si>
-    <t xml:space="preserve">Charlie	Smith</t>
+    <t xml:space="preserve">Charlie Smith</t>
   </si>
   <si>
     <t xml:space="preserve">diana.smith@example.com</t>
@@ -730,7 +733,7 @@
     <t xml:space="preserve">SMITH</t>
   </si>
   <si>
-    <t xml:space="preserve">Diana	SMITH</t>
+    <t xml:space="preserve">Diana SMITH</t>
   </si>
   <si>
     <t xml:space="preserve">eve.smith@example.com</t>
@@ -742,7 +745,7 @@
     <t xml:space="preserve">Eve</t>
   </si>
   <si>
-    <t xml:space="preserve">Eve	SMITH</t>
+    <t xml:space="preserve">Eve SMITH</t>
   </si>
   <si>
     <t xml:space="preserve">frank.smith@example.com</t>
@@ -754,7 +757,7 @@
     <t xml:space="preserve">Frank</t>
   </si>
   <si>
-    <t xml:space="preserve">Frank	SMITH</t>
+    <t xml:space="preserve">Frank SMITH</t>
   </si>
   <si>
     <t xml:space="preserve">jos.garca@example.com</t>
@@ -1605,12 +1608,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1663,8 +1672,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1680,6 +1689,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1865,20 +1934,20 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A101" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B135" activeCellId="0" sqref="B135"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E69" activeCellId="0" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="29.66"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2885,1345 +2954,1345 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>220</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>220</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>220</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>219</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>